<commit_message>
Améliration du timer + CPU
</commit_message>
<xml_diff>
--- a/Veille/FileExample/chart_aspose.xlsx
+++ b/Veille/FileExample/chart_aspose.xlsx
@@ -525,11 +525,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="10655236"/>
-        <c:axId val="28788263"/>
+        <c:axId val="53406450"/>
+        <c:axId val="10896009"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="10655236"/>
+        <c:axId val="53406450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,13 +539,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="28788263"/>
+        <c:crossAx val="10896009"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28788263"/>
+        <c:axId val="10896009"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="10655236"/>
+        <c:crossAx val="53406450"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1739,7 +1739,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02e132db-aa40-48dc-9b73-249379aa87e0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13083c83-d988-4f67-9515-3c07553c9c8f}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>

<commit_message>
Améliration du timer + CPU (#7)
</commit_message>
<xml_diff>
--- a/Veille/FileExample/chart_aspose.xlsx
+++ b/Veille/FileExample/chart_aspose.xlsx
@@ -525,11 +525,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="10655236"/>
-        <c:axId val="28788263"/>
+        <c:axId val="53406450"/>
+        <c:axId val="10896009"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="10655236"/>
+        <c:axId val="53406450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,13 +539,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="28788263"/>
+        <c:crossAx val="10896009"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28788263"/>
+        <c:axId val="10896009"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="10655236"/>
+        <c:crossAx val="53406450"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1739,7 +1739,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02e132db-aa40-48dc-9b73-249379aa87e0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13083c83-d988-4f67-9515-3c07553c9c8f}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>

</xml_diff>